<commit_message>
Minor update for clarity
</commit_message>
<xml_diff>
--- a/verif/CV32E40P/VerificationPlan/base_instruction_set/CV32E40P_instruction_exceptions.xlsx
+++ b/verif/CV32E40P/VerificationPlan/base_instruction_set/CV32E40P_instruction_exceptions.xlsx
@@ -91,10 +91,12 @@
     <t xml:space="preserve">This test case will have the code tailored to contain misaligned jump addresses.    Compressed mode "C", causes this exception to not be reachable ???</t>
   </si>
   <si>
-    <t xml:space="preserve">Demonstrate that a misaligned address jump / branch attempt will cause and exception.  Also that a misaligned address jump NOT taken does not generate and exception.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">When miss-aligned jump addresses are encountered there is an exception.  If a miss-aligned jump address is NOT taken, there is no exception.</t>
+    <t xml:space="preserve">Demonstrate that a misaligned address jump / branch attempt will cause and exception.
+Also that a misaligned address jump NOT taken does not generate and exception.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">When miss-aligned jump addresses are encountered there is an exception.  If a miss-aligned jump address is NOT taken, there is no exception.
+Demonstrate that the exception is reported on the branch/jump instruction, not the target instruction. </t>
   </si>
   <si>
     <t xml:space="preserve">ISA
@@ -564,10 +566,10 @@
   </sheetPr>
   <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -610,7 +612,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="69" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -650,7 +652,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="150" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>19</v>
       </c>

</xml_diff>